<commit_message>
Login page objects created
</commit_message>
<xml_diff>
--- a/ControlPanel/src/main/java/resources/TestCases1.xlsx
+++ b/ControlPanel/src/main/java/resources/TestCases1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -494,7 +494,9 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="3">

</xml_diff>